<commit_message>
Report editing, Cal panel date guild
- Add reference picture to report
- Change csmoScr capture position in report
- Add OBC 9.6 / Nissan OBC report
- Add date guild to csmoDate panel
</commit_message>
<xml_diff>
--- a/Leak/ext_Resources/BMW_22kW.xlsx
+++ b/Leak/ext_Resources/BMW_22kW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Leak_Format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnonymouS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76290632-1FC8-4DFD-AFCC-D25505E7DCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6608B9E4-1D9B-4D85-BE29-3EB076D3E02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="773" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cooling" sheetId="34" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>:</t>
   </si>
@@ -216,9 +216,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>CH#30  GEN4_3.7KW_ELEC</t>
   </si>
   <si>
     <t>Cal. Due Date:</t>
@@ -615,11 +612,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -671,22 +684,6 @@
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -856,8 +853,8 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr bwMode="auto">
             <a:xfrm>
-              <a:off x="662354" y="3452739"/>
-              <a:ext cx="3956538" cy="167347"/>
+              <a:off x="647700" y="3436620"/>
+              <a:ext cx="3857625" cy="169545"/>
               <a:chOff x="93" y="418"/>
               <a:chExt cx="432" cy="23"/>
             </a:xfrm>
@@ -1076,6 +1073,56 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3057525" y="7585075"/>
+          <a:ext cx="2387600" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1785,8 +1832,8 @@
   </sheetPr>
   <dimension ref="A1:AS270"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="AG12" sqref="AG12:AL13"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AU41" sqref="AU41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1947,33 +1994,33 @@
       <c r="I6" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="84" t="s">
+      <c r="J6" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="84"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
       <c r="S6" s="63"/>
       <c r="T6" s="63"/>
       <c r="U6" s="63"/>
       <c r="V6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="W6" s="87" t="s">
+      <c r="W6" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="X6" s="87"/>
-      <c r="Y6" s="87"/>
-      <c r="Z6" s="87"/>
-      <c r="AA6" s="87"/>
-      <c r="AB6" s="87"/>
-      <c r="AC6" s="87"/>
-      <c r="AD6" s="87"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
       <c r="AE6" s="63"/>
       <c r="AF6" s="63"/>
       <c r="AG6" s="11"/>
@@ -1982,12 +2029,12 @@
       <c r="AJ6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AK6" s="85"/>
-      <c r="AL6" s="85"/>
-      <c r="AM6" s="85"/>
-      <c r="AN6" s="85"/>
-      <c r="AO6" s="85"/>
-      <c r="AP6" s="85"/>
+      <c r="AK6" s="66"/>
+      <c r="AL6" s="66"/>
+      <c r="AM6" s="66"/>
+      <c r="AN6" s="66"/>
+      <c r="AO6" s="66"/>
+      <c r="AP6" s="66"/>
       <c r="AQ6" s="14"/>
     </row>
     <row r="7" spans="1:43" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2004,33 +2051,33 @@
       <c r="I7" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="66" t="s">
+      <c r="J7" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
       <c r="S7" s="63"/>
       <c r="T7" s="63"/>
       <c r="U7" s="63"/>
       <c r="V7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="W7" s="88" t="s">
+      <c r="W7" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="66"/>
-      <c r="AC7" s="66"/>
-      <c r="AD7" s="66"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="67"/>
+      <c r="Z7" s="67"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="63"/>
@@ -2039,12 +2086,12 @@
       <c r="AJ7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AK7" s="86"/>
-      <c r="AL7" s="86"/>
-      <c r="AM7" s="86"/>
-      <c r="AN7" s="86"/>
-      <c r="AO7" s="86"/>
-      <c r="AP7" s="86"/>
+      <c r="AK7" s="68"/>
+      <c r="AL7" s="68"/>
+      <c r="AM7" s="68"/>
+      <c r="AN7" s="68"/>
+      <c r="AO7" s="68"/>
+      <c r="AP7" s="68"/>
       <c r="AQ7" s="16"/>
     </row>
     <row r="8" spans="1:43" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2061,31 +2108,31 @@
       <c r="I8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
       <c r="S8" s="63"/>
       <c r="T8" s="63"/>
       <c r="U8" s="63"/>
       <c r="V8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="W8" s="66" t="s">
+      <c r="W8" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="66"/>
-      <c r="AC8" s="66"/>
-      <c r="AD8" s="66"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="67"/>
+      <c r="Z8" s="67"/>
+      <c r="AA8" s="67"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
       <c r="AE8" s="11"/>
       <c r="AF8" s="11"/>
       <c r="AG8" s="11"/>
@@ -2094,12 +2141,12 @@
       <c r="AJ8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AK8" s="67"/>
-      <c r="AL8" s="67"/>
-      <c r="AM8" s="67"/>
-      <c r="AN8" s="67"/>
-      <c r="AO8" s="67"/>
-      <c r="AP8" s="67"/>
+      <c r="AK8" s="72"/>
+      <c r="AL8" s="72"/>
+      <c r="AM8" s="72"/>
+      <c r="AN8" s="72"/>
+      <c r="AO8" s="72"/>
+      <c r="AP8" s="72"/>
       <c r="AQ8" s="14"/>
     </row>
     <row r="9" spans="1:43" s="5" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2265,7 +2312,7 @@
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
       <c r="AG12" s="90" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
@@ -2315,7 +2362,7 @@
       <c r="AE13" s="24"/>
       <c r="AF13" s="24"/>
       <c r="AG13" s="91">
-        <v>44574</v>
+        <v>44231</v>
       </c>
       <c r="AH13" s="91"/>
       <c r="AI13" s="91"/>
@@ -3329,9 +3376,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="47" t="s">
-        <v>60</v>
-      </c>
+      <c r="H35" s="47"/>
       <c r="I35" s="47"/>
       <c r="J35" s="47"/>
       <c r="K35" s="47"/>
@@ -3416,159 +3461,159 @@
     </row>
     <row r="37" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="69" t="s">
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="P37" s="70"/>
-      <c r="Q37" s="70"/>
-      <c r="R37" s="70"/>
-      <c r="S37" s="70"/>
-      <c r="T37" s="70"/>
-      <c r="U37" s="70"/>
-      <c r="V37" s="70"/>
-      <c r="W37" s="70"/>
-      <c r="X37" s="70"/>
-      <c r="Y37" s="70"/>
-      <c r="Z37" s="70"/>
-      <c r="AA37" s="70"/>
-      <c r="AB37" s="70"/>
-      <c r="AC37" s="70"/>
-      <c r="AD37" s="70"/>
-      <c r="AE37" s="70"/>
-      <c r="AF37" s="70"/>
-      <c r="AG37" s="70"/>
-      <c r="AH37" s="70"/>
-      <c r="AI37" s="70"/>
-      <c r="AJ37" s="70"/>
-      <c r="AK37" s="70"/>
-      <c r="AL37" s="70"/>
-      <c r="AM37" s="70"/>
-      <c r="AN37" s="70"/>
-      <c r="AO37" s="70"/>
-      <c r="AP37" s="71"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="75"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="75"/>
+      <c r="U37" s="75"/>
+      <c r="V37" s="75"/>
+      <c r="W37" s="75"/>
+      <c r="X37" s="75"/>
+      <c r="Y37" s="75"/>
+      <c r="Z37" s="75"/>
+      <c r="AA37" s="75"/>
+      <c r="AB37" s="75"/>
+      <c r="AC37" s="75"/>
+      <c r="AD37" s="75"/>
+      <c r="AE37" s="75"/>
+      <c r="AF37" s="75"/>
+      <c r="AG37" s="75"/>
+      <c r="AH37" s="75"/>
+      <c r="AI37" s="75"/>
+      <c r="AJ37" s="75"/>
+      <c r="AK37" s="75"/>
+      <c r="AL37" s="75"/>
+      <c r="AM37" s="75"/>
+      <c r="AN37" s="75"/>
+      <c r="AO37" s="75"/>
+      <c r="AP37" s="76"/>
       <c r="AQ37" s="33"/>
     </row>
     <row r="38" spans="1:45" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="31"/>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="72" t="s">
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="P38" s="73"/>
-      <c r="Q38" s="73"/>
-      <c r="R38" s="73"/>
-      <c r="S38" s="73"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="72" t="s">
+      <c r="P38" s="78"/>
+      <c r="Q38" s="78"/>
+      <c r="R38" s="78"/>
+      <c r="S38" s="78"/>
+      <c r="T38" s="79"/>
+      <c r="U38" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="V38" s="73"/>
-      <c r="W38" s="73"/>
-      <c r="X38" s="73"/>
-      <c r="Y38" s="73"/>
-      <c r="Z38" s="73"/>
-      <c r="AA38" s="74"/>
-      <c r="AB38" s="75" t="s">
+      <c r="V38" s="78"/>
+      <c r="W38" s="78"/>
+      <c r="X38" s="78"/>
+      <c r="Y38" s="78"/>
+      <c r="Z38" s="78"/>
+      <c r="AA38" s="79"/>
+      <c r="AB38" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="AC38" s="73"/>
-      <c r="AD38" s="73"/>
-      <c r="AE38" s="73"/>
-      <c r="AF38" s="73"/>
-      <c r="AG38" s="74"/>
-      <c r="AH38" s="76" t="s">
+      <c r="AC38" s="78"/>
+      <c r="AD38" s="78"/>
+      <c r="AE38" s="78"/>
+      <c r="AF38" s="78"/>
+      <c r="AG38" s="79"/>
+      <c r="AH38" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="AI38" s="77"/>
-      <c r="AJ38" s="77"/>
-      <c r="AK38" s="77"/>
-      <c r="AL38" s="77"/>
-      <c r="AM38" s="68" t="s">
+      <c r="AI38" s="82"/>
+      <c r="AJ38" s="82"/>
+      <c r="AK38" s="82"/>
+      <c r="AL38" s="82"/>
+      <c r="AM38" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="AN38" s="68"/>
-      <c r="AO38" s="68"/>
-      <c r="AP38" s="68"/>
+      <c r="AN38" s="73"/>
+      <c r="AO38" s="73"/>
+      <c r="AP38" s="73"/>
       <c r="AQ38" s="33"/>
     </row>
     <row r="39" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="79"/>
-      <c r="O39" s="79" t="s">
+      <c r="B39" s="83"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="84"/>
+      <c r="K39" s="84"/>
+      <c r="L39" s="84"/>
+      <c r="M39" s="84"/>
+      <c r="N39" s="84"/>
+      <c r="O39" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="P39" s="79"/>
-      <c r="Q39" s="79"/>
-      <c r="R39" s="79"/>
-      <c r="S39" s="79"/>
-      <c r="T39" s="79"/>
-      <c r="U39" s="79" t="s">
+      <c r="P39" s="84"/>
+      <c r="Q39" s="84"/>
+      <c r="R39" s="84"/>
+      <c r="S39" s="84"/>
+      <c r="T39" s="84"/>
+      <c r="U39" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="V39" s="79"/>
-      <c r="W39" s="79"/>
-      <c r="X39" s="79"/>
-      <c r="Y39" s="79"/>
-      <c r="Z39" s="79"/>
-      <c r="AA39" s="79"/>
-      <c r="AB39" s="80" t="s">
+      <c r="V39" s="84"/>
+      <c r="W39" s="84"/>
+      <c r="X39" s="84"/>
+      <c r="Y39" s="84"/>
+      <c r="Z39" s="84"/>
+      <c r="AA39" s="84"/>
+      <c r="AB39" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="AC39" s="81"/>
-      <c r="AD39" s="81"/>
-      <c r="AE39" s="81"/>
-      <c r="AF39" s="81"/>
-      <c r="AG39" s="81"/>
-      <c r="AH39" s="82"/>
-      <c r="AI39" s="83"/>
-      <c r="AJ39" s="83"/>
-      <c r="AK39" s="83"/>
-      <c r="AL39" s="83"/>
-      <c r="AM39" s="65" t="s">
+      <c r="AC39" s="86"/>
+      <c r="AD39" s="86"/>
+      <c r="AE39" s="86"/>
+      <c r="AF39" s="86"/>
+      <c r="AG39" s="86"/>
+      <c r="AH39" s="87"/>
+      <c r="AI39" s="88"/>
+      <c r="AJ39" s="88"/>
+      <c r="AK39" s="88"/>
+      <c r="AL39" s="88"/>
+      <c r="AM39" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="AN39" s="65"/>
-      <c r="AO39" s="65"/>
-      <c r="AP39" s="65"/>
+      <c r="AN39" s="71"/>
+      <c r="AO39" s="71"/>
+      <c r="AP39" s="71"/>
       <c r="AQ39" s="33"/>
     </row>
     <row r="40" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4517,12 +4562,6 @@
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="AG13:AL13"/>
-    <mergeCell ref="J6:R6"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="J7:R7"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="W7:AD7"/>
     <mergeCell ref="AM39:AP39"/>
     <mergeCell ref="J8:R8"/>
     <mergeCell ref="AK8:AP8"/>
@@ -4539,6 +4578,12 @@
     <mergeCell ref="U39:AA39"/>
     <mergeCell ref="AB39:AG39"/>
     <mergeCell ref="AH39:AL39"/>
+    <mergeCell ref="J6:R6"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="J7:R7"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="W7:AD7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="M28 G28:K28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -4655,8 +4700,8 @@
   </sheetPr>
   <dimension ref="A1:AS270"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AU21" sqref="AU21"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AM39" sqref="AM39:AP39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4813,44 +4858,44 @@
       <c r="I6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="84" t="str">
+      <c r="J6" s="65" t="str">
         <f>Cooling!J6</f>
         <v>ECD18020003</v>
       </c>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="84"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
       <c r="V6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="W6" s="84" t="str">
+      <c r="W6" s="65" t="str">
         <f>Cooling!W6</f>
         <v>-</v>
       </c>
-      <c r="X6" s="84"/>
-      <c r="Y6" s="84"/>
-      <c r="Z6" s="84"/>
-      <c r="AA6" s="84"/>
-      <c r="AB6" s="84"/>
-      <c r="AC6" s="84"/>
-      <c r="AD6" s="84"/>
+      <c r="X6" s="65"/>
+      <c r="Y6" s="65"/>
+      <c r="Z6" s="65"/>
+      <c r="AA6" s="65"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="65"/>
+      <c r="AD6" s="65"/>
       <c r="AG6" s="11"/>
       <c r="AH6" s="11"/>
       <c r="AI6" s="11"/>
       <c r="AJ6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AK6" s="85"/>
-      <c r="AL6" s="85"/>
-      <c r="AM6" s="85"/>
-      <c r="AN6" s="85"/>
-      <c r="AO6" s="85"/>
-      <c r="AP6" s="85"/>
+      <c r="AK6" s="66"/>
+      <c r="AL6" s="66"/>
+      <c r="AM6" s="66"/>
+      <c r="AN6" s="66"/>
+      <c r="AO6" s="66"/>
+      <c r="AP6" s="66"/>
       <c r="AQ6" s="14"/>
     </row>
     <row r="7" spans="1:43" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4865,32 +4910,32 @@
       <c r="I7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="66" t="str">
+      <c r="J7" s="67" t="str">
         <f>Cooling!J7</f>
         <v>BMW</v>
       </c>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
       <c r="V7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="W7" s="66" t="str">
+      <c r="W7" s="67" t="str">
         <f>Cooling!W7</f>
         <v>-</v>
       </c>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="66"/>
-      <c r="AC7" s="66"/>
-      <c r="AD7" s="66"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="67"/>
+      <c r="Z7" s="67"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AH7" s="11"/>
@@ -4898,12 +4943,12 @@
       <c r="AJ7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AK7" s="86"/>
-      <c r="AL7" s="86"/>
-      <c r="AM7" s="86"/>
-      <c r="AN7" s="86"/>
-      <c r="AO7" s="86"/>
-      <c r="AP7" s="86"/>
+      <c r="AK7" s="68"/>
+      <c r="AL7" s="68"/>
+      <c r="AM7" s="68"/>
+      <c r="AN7" s="68"/>
+      <c r="AO7" s="68"/>
+      <c r="AP7" s="68"/>
       <c r="AQ7" s="16"/>
     </row>
     <row r="8" spans="1:43" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4920,29 +4965,29 @@
       <c r="I8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
       <c r="V8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="W8" s="66" t="str">
+      <c r="W8" s="67" t="str">
         <f>Cooling!W8</f>
         <v>-</v>
       </c>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="66"/>
-      <c r="AC8" s="66"/>
-      <c r="AD8" s="66"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="67"/>
+      <c r="Z8" s="67"/>
+      <c r="AA8" s="67"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
       <c r="AE8" s="11"/>
       <c r="AF8" s="11"/>
       <c r="AG8" s="11"/>
@@ -4951,12 +4996,12 @@
       <c r="AJ8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AK8" s="67"/>
-      <c r="AL8" s="67"/>
-      <c r="AM8" s="67"/>
-      <c r="AN8" s="67"/>
-      <c r="AO8" s="67"/>
-      <c r="AP8" s="67"/>
+      <c r="AK8" s="72"/>
+      <c r="AL8" s="72"/>
+      <c r="AM8" s="72"/>
+      <c r="AN8" s="72"/>
+      <c r="AO8" s="72"/>
+      <c r="AP8" s="72"/>
       <c r="AQ8" s="14"/>
     </row>
     <row r="9" spans="1:43" s="5" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5119,7 +5164,7 @@
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
       <c r="AG12" s="90" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
@@ -5169,7 +5214,7 @@
       <c r="AE13" s="24"/>
       <c r="AF13" s="24"/>
       <c r="AG13" s="91">
-        <v>44574</v>
+        <v>44231</v>
       </c>
       <c r="AH13" s="91"/>
       <c r="AI13" s="91"/>
@@ -6254,159 +6299,157 @@
     </row>
     <row r="37" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="69" t="s">
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="P37" s="70"/>
-      <c r="Q37" s="70"/>
-      <c r="R37" s="70"/>
-      <c r="S37" s="70"/>
-      <c r="T37" s="70"/>
-      <c r="U37" s="70"/>
-      <c r="V37" s="70"/>
-      <c r="W37" s="70"/>
-      <c r="X37" s="70"/>
-      <c r="Y37" s="70"/>
-      <c r="Z37" s="70"/>
-      <c r="AA37" s="70"/>
-      <c r="AB37" s="70"/>
-      <c r="AC37" s="70"/>
-      <c r="AD37" s="70"/>
-      <c r="AE37" s="70"/>
-      <c r="AF37" s="70"/>
-      <c r="AG37" s="70"/>
-      <c r="AH37" s="70"/>
-      <c r="AI37" s="70"/>
-      <c r="AJ37" s="70"/>
-      <c r="AK37" s="70"/>
-      <c r="AL37" s="70"/>
-      <c r="AM37" s="70"/>
-      <c r="AN37" s="70"/>
-      <c r="AO37" s="70"/>
-      <c r="AP37" s="71"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="75"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="75"/>
+      <c r="U37" s="75"/>
+      <c r="V37" s="75"/>
+      <c r="W37" s="75"/>
+      <c r="X37" s="75"/>
+      <c r="Y37" s="75"/>
+      <c r="Z37" s="75"/>
+      <c r="AA37" s="75"/>
+      <c r="AB37" s="75"/>
+      <c r="AC37" s="75"/>
+      <c r="AD37" s="75"/>
+      <c r="AE37" s="75"/>
+      <c r="AF37" s="75"/>
+      <c r="AG37" s="75"/>
+      <c r="AH37" s="75"/>
+      <c r="AI37" s="75"/>
+      <c r="AJ37" s="75"/>
+      <c r="AK37" s="75"/>
+      <c r="AL37" s="75"/>
+      <c r="AM37" s="75"/>
+      <c r="AN37" s="75"/>
+      <c r="AO37" s="75"/>
+      <c r="AP37" s="76"/>
       <c r="AQ37" s="33"/>
     </row>
     <row r="38" spans="1:45" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="31"/>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="72" t="s">
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="P38" s="73"/>
-      <c r="Q38" s="73"/>
-      <c r="R38" s="73"/>
-      <c r="S38" s="73"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="72" t="s">
+      <c r="P38" s="78"/>
+      <c r="Q38" s="78"/>
+      <c r="R38" s="78"/>
+      <c r="S38" s="78"/>
+      <c r="T38" s="79"/>
+      <c r="U38" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="V38" s="73"/>
-      <c r="W38" s="73"/>
-      <c r="X38" s="73"/>
-      <c r="Y38" s="73"/>
-      <c r="Z38" s="73"/>
-      <c r="AA38" s="74"/>
-      <c r="AB38" s="72" t="s">
+      <c r="V38" s="78"/>
+      <c r="W38" s="78"/>
+      <c r="X38" s="78"/>
+      <c r="Y38" s="78"/>
+      <c r="Z38" s="78"/>
+      <c r="AA38" s="79"/>
+      <c r="AB38" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="AC38" s="73"/>
-      <c r="AD38" s="73"/>
-      <c r="AE38" s="73"/>
-      <c r="AF38" s="73"/>
-      <c r="AG38" s="74"/>
-      <c r="AH38" s="76" t="s">
+      <c r="AC38" s="78"/>
+      <c r="AD38" s="78"/>
+      <c r="AE38" s="78"/>
+      <c r="AF38" s="78"/>
+      <c r="AG38" s="79"/>
+      <c r="AH38" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="AI38" s="77"/>
-      <c r="AJ38" s="77"/>
-      <c r="AK38" s="77"/>
-      <c r="AL38" s="77"/>
-      <c r="AM38" s="68" t="s">
+      <c r="AI38" s="82"/>
+      <c r="AJ38" s="82"/>
+      <c r="AK38" s="82"/>
+      <c r="AL38" s="82"/>
+      <c r="AM38" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="AN38" s="68"/>
-      <c r="AO38" s="68"/>
-      <c r="AP38" s="68"/>
+      <c r="AN38" s="73"/>
+      <c r="AO38" s="73"/>
+      <c r="AP38" s="73"/>
       <c r="AQ38" s="33"/>
     </row>
     <row r="39" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="79"/>
-      <c r="O39" s="79" t="s">
+      <c r="B39" s="83"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="84"/>
+      <c r="K39" s="84"/>
+      <c r="L39" s="84"/>
+      <c r="M39" s="84"/>
+      <c r="N39" s="84"/>
+      <c r="O39" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="P39" s="79"/>
-      <c r="Q39" s="79"/>
-      <c r="R39" s="79"/>
-      <c r="S39" s="79"/>
-      <c r="T39" s="79"/>
-      <c r="U39" s="79" t="s">
+      <c r="P39" s="84"/>
+      <c r="Q39" s="84"/>
+      <c r="R39" s="84"/>
+      <c r="S39" s="84"/>
+      <c r="T39" s="84"/>
+      <c r="U39" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="V39" s="79"/>
-      <c r="W39" s="79"/>
-      <c r="X39" s="79"/>
-      <c r="Y39" s="79"/>
-      <c r="Z39" s="79"/>
-      <c r="AA39" s="79"/>
-      <c r="AB39" s="80" t="s">
+      <c r="V39" s="84"/>
+      <c r="W39" s="84"/>
+      <c r="X39" s="84"/>
+      <c r="Y39" s="84"/>
+      <c r="Z39" s="84"/>
+      <c r="AA39" s="84"/>
+      <c r="AB39" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="AC39" s="81"/>
-      <c r="AD39" s="81"/>
-      <c r="AE39" s="81"/>
-      <c r="AF39" s="81"/>
-      <c r="AG39" s="81"/>
+      <c r="AC39" s="86"/>
+      <c r="AD39" s="86"/>
+      <c r="AE39" s="86"/>
+      <c r="AF39" s="86"/>
+      <c r="AG39" s="86"/>
       <c r="AH39" s="89"/>
       <c r="AI39" s="89"/>
       <c r="AJ39" s="89"/>
       <c r="AK39" s="89"/>
       <c r="AL39" s="89"/>
-      <c r="AM39" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN39" s="65"/>
-      <c r="AO39" s="65"/>
-      <c r="AP39" s="65"/>
+      <c r="AM39" s="71"/>
+      <c r="AN39" s="71"/>
+      <c r="AO39" s="71"/>
+      <c r="AP39" s="71"/>
       <c r="AQ39" s="33"/>
     </row>
     <row r="40" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7275,12 +7318,12 @@
     <row r="270" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="J6:R6"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="J7:R7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AM39:AP39"/>
+    <mergeCell ref="B39:N39"/>
+    <mergeCell ref="O39:T39"/>
+    <mergeCell ref="U39:AA39"/>
+    <mergeCell ref="AB39:AG39"/>
+    <mergeCell ref="AH39:AL39"/>
     <mergeCell ref="J8:R8"/>
     <mergeCell ref="W8:AD8"/>
     <mergeCell ref="AK8:AP8"/>
@@ -7292,12 +7335,12 @@
     <mergeCell ref="AH38:AL38"/>
     <mergeCell ref="AM38:AP38"/>
     <mergeCell ref="AG13:AL13"/>
-    <mergeCell ref="AM39:AP39"/>
-    <mergeCell ref="B39:N39"/>
-    <mergeCell ref="O39:T39"/>
-    <mergeCell ref="U39:AA39"/>
-    <mergeCell ref="AB39:AG39"/>
-    <mergeCell ref="AH39:AL39"/>
+    <mergeCell ref="J6:R6"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="J7:R7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="AK7:AP7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="N28 H28:L28" xr:uid="{00000000-0002-0000-0100-000000000000}"/>

</xml_diff>